<commit_message>
add update data feature
</commit_message>
<xml_diff>
--- a/resource/in_house_template_input_database.xlsx
+++ b/resource/in_house_template_input_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hafiyyankisaragi/Development/Python/Toyota-PMBD/dashboard-MSP/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0734C031-4D47-824C-92D3-5E5CEE8B0CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36302201-31FD-7344-ADD0-DBC35209BC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="1780" windowWidth="27240" windowHeight="16040" xr2:uid="{DCCCB11C-156F-DE44-9AC4-8ACD75CC4C69}"/>
   </bookViews>
@@ -487,7 +487,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>